<commit_message>
changed submission form message
</commit_message>
<xml_diff>
--- a/backend/visitor_data.xlsx
+++ b/backend/visitor_data.xlsx
@@ -1,41 +1,143 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siman\OneDrive\Desktop\ReactProjects\church-visitor-form\backend\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5652F6EF-9793-4C40-B173-C632DB728D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Visitors" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>College Student</t>
+  </si>
+  <si>
+    <t>Student Status</t>
+  </si>
+  <si>
+    <t>How Heard</t>
+  </si>
+  <si>
+    <t>Membership</t>
+  </si>
+  <si>
+    <t>Prayer</t>
+  </si>
+  <si>
+    <t>Pastor Visit</t>
+  </si>
+  <si>
+    <t>More Info</t>
+  </si>
+  <si>
+    <t>Sima</t>
+  </si>
+  <si>
+    <t>sima@gmail.com</t>
+  </si>
+  <si>
+    <t>13202246421</t>
+  </si>
+  <si>
+    <t>Manassas, Virginia, 20111</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Friend</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>About my faith</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>2040 15th St N</t>
+  </si>
+  <si>
+    <t>Graduate</t>
+  </si>
+  <si>
+    <t>classmate</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>paul@gmail.com</t>
+  </si>
+  <si>
+    <t>914 15th St N</t>
+  </si>
+  <si>
+    <t>Met a church member</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>david@gmail.com</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>1546 12th ST N</t>
+  </si>
+  <si>
+    <t>Senior</t>
+  </si>
+  <si>
+    <t>Friends</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +167,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,120 +506,195 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Email</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Phone</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Address</v>
-      </c>
-      <c r="E1" t="str">
-        <v>College Student</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Student Status</v>
-      </c>
-      <c r="G1" t="str">
-        <v>How Heard</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Membership</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Prayer</v>
-      </c>
-      <c r="J1" t="str">
-        <v>Pastor Visit</v>
-      </c>
-      <c r="K1" t="str">
-        <v>More Info</v>
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Sima</v>
-      </c>
-      <c r="B2" t="str">
-        <v>sima@gmail.com</v>
-      </c>
-      <c r="C2" t="str">
-        <v>13202246421</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Manassas, Virginia, 20111</v>
-      </c>
-      <c r="E2" t="str">
-        <v>no</v>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v>Friend</v>
-      </c>
-      <c r="H2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="I2" t="str">
-        <v>About my faith</v>
-      </c>
-      <c r="J2" t="str">
-        <v>yes</v>
-      </c>
-      <c r="K2" t="str">
-        <v>yes</v>
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>John Doe</v>
-      </c>
-      <c r="B3" t="str">
-        <v>john@gmail.com</v>
-      </c>
-      <c r="C3" t="str">
-        <v>12345678</v>
-      </c>
-      <c r="D3" t="str">
-        <v>2040 15th St N</v>
-      </c>
-      <c r="E3" t="str">
-        <v>yes</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Graduate</v>
-      </c>
-      <c r="G3" t="str">
-        <v>classmate</v>
-      </c>
-      <c r="H3" t="str">
-        <v>no</v>
-      </c>
-      <c r="I3" t="str">
-        <v>N/A</v>
-      </c>
-      <c r="J3" t="str">
-        <v>no</v>
-      </c>
-      <c r="K3" t="str">
-        <v>no</v>
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
+    <ignoredError sqref="A1:K5" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>